<commit_message>
I've learned more topics
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E2F4420-1E64-45FF-8EB9-6025315BCCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E332B3-1916-43AB-8BDA-C13327E688E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1A1ABF10-E896-4C32-A5C9-4992F1642E40}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>DSA</t>
   </si>
@@ -66,7 +66,13 @@
     <t>Stack using Array</t>
   </si>
   <si>
-    <t>HashMap or HashTable</t>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <t>Tree</t>
   </si>
 </sst>
 </file>
@@ -145,13 +151,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59170B4-9C14-4ABF-B469-574371093CDB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,96 +485,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Have learned more topics
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E332B3-1916-43AB-8BDA-C13327E688E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4F12B2-26D0-4E86-8D55-A97E50BFD5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1A1ABF10-E896-4C32-A5C9-4992F1642E40}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>DSA</t>
   </si>
@@ -73,13 +73,34 @@
   </si>
   <si>
     <t>Tree</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Linear Search</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Bubble Sort</t>
+  </si>
+  <si>
+    <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +116,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,8 +150,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -145,18 +180,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59170B4-9C14-4ABF-B469-574371093CDB}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,30 +556,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -516,7 +585,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -524,7 +593,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -532,7 +601,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -540,7 +609,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -548,7 +617,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -556,7 +625,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -564,7 +633,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -572,7 +641,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -580,7 +649,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -588,21 +657,83 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>